<commit_message>
Conserto do erro com o rótulo da coluna 2050 nas tabelas e retirada das linhas com total das tabelas
</commit_message>
<xml_diff>
--- a/04_PipelineTCU/constants/Cenarios_PNE/01. Estagnaç╞o.xlsx
+++ b/04_PipelineTCU/constants/Cenarios_PNE/01. Estagnaç╞o.xlsx
@@ -430,7 +430,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -454,8 +454,10 @@
           <t>2040</t>
         </is>
       </c>
-      <c r="E1" s="1" t="n">
-        <v>269.0255923131356</v>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>2050</t>
+        </is>
       </c>
     </row>
     <row r="2">
@@ -665,25 +667,6 @@
       </c>
       <c r="E12" t="n">
         <v>8395</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="1" t="inlineStr">
-        <is>
-          <t>Total</t>
-        </is>
-      </c>
-      <c r="B13" t="n">
-        <v>135896</v>
-      </c>
-      <c r="C13" t="n">
-        <v>168751</v>
-      </c>
-      <c r="D13" t="n">
-        <v>166976</v>
-      </c>
-      <c r="E13" t="n">
-        <v>170832</v>
       </c>
     </row>
   </sheetData>
@@ -697,7 +680,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -721,8 +704,10 @@
           <t>2040</t>
         </is>
       </c>
-      <c r="E1" s="1" t="n">
-        <v>269.0255923131356</v>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>2050</t>
+        </is>
       </c>
     </row>
     <row r="2">
@@ -932,25 +917,6 @@
       </c>
       <c r="E12" t="n">
         <v>3664</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="1" t="inlineStr">
-        <is>
-          <t>Total</t>
-        </is>
-      </c>
-      <c r="B13" t="n">
-        <v>67082</v>
-      </c>
-      <c r="C13" t="n">
-        <v>73640</v>
-      </c>
-      <c r="D13" t="n">
-        <v>75575</v>
-      </c>
-      <c r="E13" t="n">
-        <v>76443</v>
       </c>
     </row>
   </sheetData>
@@ -964,7 +930,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -988,8 +954,10 @@
           <t>2040</t>
         </is>
       </c>
-      <c r="E1" s="1" t="n">
-        <v>269.0255923131356</v>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>2050</t>
+        </is>
       </c>
     </row>
     <row r="2">
@@ -1199,25 +1167,6 @@
       </c>
       <c r="E12" t="n">
         <v>1248</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="1" t="inlineStr">
-        <is>
-          <t>Total</t>
-        </is>
-      </c>
-      <c r="B13" t="n">
-        <v>88476</v>
-      </c>
-      <c r="C13" t="n">
-        <v>104754</v>
-      </c>
-      <c r="D13" t="n">
-        <v>109961</v>
-      </c>
-      <c r="E13" t="n">
-        <v>110303</v>
       </c>
     </row>
   </sheetData>
@@ -1231,7 +1180,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1255,8 +1204,10 @@
           <t>2031-2040</t>
         </is>
       </c>
-      <c r="E1" s="1" t="n">
-        <v>269.0255923131356</v>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>2041-2050</t>
+        </is>
       </c>
     </row>
     <row r="2">
@@ -1466,25 +1417,6 @@
       </c>
       <c r="E12" t="n">
         <v>2870</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="1" t="inlineStr">
-        <is>
-          <t>Total</t>
-        </is>
-      </c>
-      <c r="B13" t="n">
-        <v>0</v>
-      </c>
-      <c r="C13" t="n">
-        <v>32854</v>
-      </c>
-      <c r="D13" t="n">
-        <v>-1774</v>
-      </c>
-      <c r="E13" t="n">
-        <v>3855</v>
       </c>
     </row>
   </sheetData>
@@ -1522,8 +1454,10 @@
           <t>2040</t>
         </is>
       </c>
-      <c r="E1" s="1" t="n">
-        <v>269.0255923131356</v>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>2050</t>
+        </is>
       </c>
     </row>
     <row r="2">
@@ -1594,7 +1528,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1629,16 +1563,6 @@
         <v>38</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" s="1" t="inlineStr">
-        <is>
-          <t>Total</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
-        <v>251</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Colocando header nos gráficos
</commit_message>
<xml_diff>
--- a/04_PipelineTCU/constants/Cenarios_PNE/01. Estagnaç╞o.xlsx
+++ b/04_PipelineTCU/constants/Cenarios_PNE/01. Estagnaç╞o.xlsx
@@ -439,6 +439,11 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Fonte/Tecnologia</t>
+        </is>
+      </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
           <t>2015</t>
@@ -461,7 +466,7 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="inlineStr">
+      <c r="A2" t="inlineStr">
         <is>
           <t>Hidro</t>
         </is>
@@ -480,9 +485,9 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="inlineStr">
-        <is>
-          <t>Gas Natural</t>
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Gás Natural</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -499,9 +504,9 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="1" t="inlineStr">
-        <is>
-          <t>Carvao</t>
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Carvão</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -518,7 +523,7 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="1" t="inlineStr">
+      <c r="A5" t="inlineStr">
         <is>
           <t>Nuclear</t>
         </is>
@@ -537,9 +542,9 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="1" t="inlineStr">
-        <is>
-          <t>Oleos Comb</t>
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Óleos Comb</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -556,7 +561,7 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="1" t="inlineStr">
+      <c r="A7" t="inlineStr">
         <is>
           <t>Biomassa</t>
         </is>
@@ -575,9 +580,9 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="1" t="inlineStr">
-        <is>
-          <t>Eolica</t>
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Eólica</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -594,7 +599,7 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="1" t="inlineStr">
+      <c r="A9" t="inlineStr">
         <is>
           <t>Solar</t>
         </is>
@@ -613,7 +618,7 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="1" t="inlineStr">
+      <c r="A10" t="inlineStr">
         <is>
           <t>Outros</t>
         </is>
@@ -632,9 +637,9 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="1" t="inlineStr">
-        <is>
-          <t>Pot Compl</t>
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Pot. Compl.</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -651,7 +656,7 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="1" t="inlineStr">
+      <c r="A12" t="inlineStr">
         <is>
           <t>GD</t>
         </is>
@@ -689,6 +694,11 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Fonte/Tecnologia</t>
+        </is>
+      </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
           <t>2015</t>
@@ -711,7 +721,7 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="inlineStr">
+      <c r="A2" t="inlineStr">
         <is>
           <t>Hidro</t>
         </is>
@@ -730,9 +740,9 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="inlineStr">
-        <is>
-          <t>Gas Natural</t>
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Gás Natural</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -749,9 +759,9 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="1" t="inlineStr">
-        <is>
-          <t>Carvao</t>
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Carvão</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -768,7 +778,7 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="1" t="inlineStr">
+      <c r="A5" t="inlineStr">
         <is>
           <t>Nuclear</t>
         </is>
@@ -787,9 +797,9 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="1" t="inlineStr">
-        <is>
-          <t>Oleos Comb</t>
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Óleos Comb</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -806,7 +816,7 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="1" t="inlineStr">
+      <c r="A7" t="inlineStr">
         <is>
           <t>Biomassa</t>
         </is>
@@ -825,9 +835,9 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="1" t="inlineStr">
-        <is>
-          <t>Eolica</t>
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Eólica</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -844,7 +854,7 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="1" t="inlineStr">
+      <c r="A9" t="inlineStr">
         <is>
           <t>Solar</t>
         </is>
@@ -863,7 +873,7 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="1" t="inlineStr">
+      <c r="A10" t="inlineStr">
         <is>
           <t>Outros</t>
         </is>
@@ -882,9 +892,9 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="1" t="inlineStr">
-        <is>
-          <t>Pot Compl</t>
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Pot. Compl.</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -901,7 +911,7 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="1" t="inlineStr">
+      <c r="A12" t="inlineStr">
         <is>
           <t>GD</t>
         </is>
@@ -939,6 +949,11 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Fonte/Tecnologia</t>
+        </is>
+      </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
           <t>2015</t>
@@ -961,7 +976,7 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="inlineStr">
+      <c r="A2" t="inlineStr">
         <is>
           <t>Hidro</t>
         </is>
@@ -980,9 +995,9 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="inlineStr">
-        <is>
-          <t>Gas Natural</t>
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Gás Natural</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -999,9 +1014,9 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="1" t="inlineStr">
-        <is>
-          <t>Carvao</t>
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Carvão</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -1018,7 +1033,7 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="1" t="inlineStr">
+      <c r="A5" t="inlineStr">
         <is>
           <t>Nuclear</t>
         </is>
@@ -1037,9 +1052,9 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="1" t="inlineStr">
-        <is>
-          <t>Oleos Comb</t>
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Óleos Comb</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -1056,7 +1071,7 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="1" t="inlineStr">
+      <c r="A7" t="inlineStr">
         <is>
           <t>Biomassa</t>
         </is>
@@ -1075,9 +1090,9 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="1" t="inlineStr">
-        <is>
-          <t>Eolica</t>
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Eólica</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -1094,7 +1109,7 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="1" t="inlineStr">
+      <c r="A9" t="inlineStr">
         <is>
           <t>Solar</t>
         </is>
@@ -1113,7 +1128,7 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="1" t="inlineStr">
+      <c r="A10" t="inlineStr">
         <is>
           <t>Outros</t>
         </is>
@@ -1132,9 +1147,9 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="1" t="inlineStr">
-        <is>
-          <t>Pot Compl</t>
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Pot. Compl.</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -1151,7 +1166,7 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="1" t="inlineStr">
+      <c r="A12" t="inlineStr">
         <is>
           <t>GD</t>
         </is>
@@ -1189,6 +1204,11 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Fonte/Tecnologia</t>
+        </is>
+      </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
           <t>2015</t>
@@ -1211,7 +1231,7 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="inlineStr">
+      <c r="A2" t="inlineStr">
         <is>
           <t>Hidro</t>
         </is>
@@ -1230,9 +1250,9 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="inlineStr">
-        <is>
-          <t>Gas Natural</t>
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Gás Natural</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -1249,9 +1269,9 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="1" t="inlineStr">
-        <is>
-          <t>Carvao</t>
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Carvão</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -1268,7 +1288,7 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="1" t="inlineStr">
+      <c r="A5" t="inlineStr">
         <is>
           <t>Nuclear</t>
         </is>
@@ -1287,9 +1307,9 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="1" t="inlineStr">
-        <is>
-          <t>Oleos Comb</t>
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Óleos Comb</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -1306,7 +1326,7 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="1" t="inlineStr">
+      <c r="A7" t="inlineStr">
         <is>
           <t>Biomassa</t>
         </is>
@@ -1325,9 +1345,9 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="1" t="inlineStr">
-        <is>
-          <t>Eolica</t>
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Eólica</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -1344,7 +1364,7 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="1" t="inlineStr">
+      <c r="A9" t="inlineStr">
         <is>
           <t>Solar</t>
         </is>
@@ -1363,7 +1383,7 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="1" t="inlineStr">
+      <c r="A10" t="inlineStr">
         <is>
           <t>Outros</t>
         </is>
@@ -1382,9 +1402,9 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="1" t="inlineStr">
-        <is>
-          <t>Pot Compl</t>
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Pot. Compl.</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -1401,7 +1421,7 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="1" t="inlineStr">
+      <c r="A12" t="inlineStr">
         <is>
           <t>GD</t>
         </is>
@@ -1430,7 +1450,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1439,6 +1459,11 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Período</t>
+        </is>
+      </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
           <t>2015</t>
@@ -1461,9 +1486,9 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="inlineStr">
-        <is>
-          <t>P Medio</t>
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>P.Médio</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -1480,9 +1505,9 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="inlineStr">
-        <is>
-          <t>P Critico</t>
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>P.Crítico</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -1496,25 +1521,6 @@
       </c>
       <c r="E3" t="n">
         <v>5</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="1" t="inlineStr">
-        <is>
-          <t>Teto</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
-        <v>10000000</v>
-      </c>
-      <c r="C4" t="n">
-        <v>10000000</v>
-      </c>
-      <c r="D4" t="n">
-        <v>10000000</v>
-      </c>
-      <c r="E4" t="n">
-        <v>10000000</v>
       </c>
     </row>
   </sheetData>
@@ -1537,30 +1543,35 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Tipo Expansão</t>
+        </is>
+      </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Custo</t>
+          <t>2015</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="inlineStr">
-        <is>
-          <t>Expansao Centralizada</t>
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Expansão Centralizada</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>213</v>
+        <v>169</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="inlineStr">
-        <is>
-          <t>Expansao por GD</t>
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Expansão por GD</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>38</v>
+        <v>99</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
(#33) Alteração nos rótulos da tabela para já transformar a primeira linha em cabeçalho automaticamente no power bi
</commit_message>
<xml_diff>
--- a/04_PipelineTCU/constants/Cenarios_PNE/01. Estagnaç╞o.xlsx
+++ b/04_PipelineTCU/constants/Cenarios_PNE/01. Estagnaç╞o.xlsx
@@ -446,22 +446,22 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>2015</t>
+          <t>Ano 2015</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>2030</t>
+          <t>Ano 2030</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>2040</t>
+          <t>Ano 2040</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>2050</t>
+          <t>Ano 2050</t>
         </is>
       </c>
     </row>
@@ -701,22 +701,22 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>2015</t>
+          <t>Ano 2015</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>2030</t>
+          <t>Ano 2030</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>2040</t>
+          <t>Ano 2040</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>2050</t>
+          <t>Ano 2050</t>
         </is>
       </c>
     </row>
@@ -956,22 +956,22 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>2015</t>
+          <t>Ano 2015</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>2030</t>
+          <t>Ano 2030</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>2040</t>
+          <t>Ano 2040</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>2050</t>
+          <t>Ano 2050</t>
         </is>
       </c>
     </row>
@@ -1211,22 +1211,22 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>2015</t>
+          <t>Intervalo 2015</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>2015-2030</t>
+          <t>Intervalo 2015-2030</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>2031-2040</t>
+          <t>Intervalo 2031-2040</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>2041-2050</t>
+          <t>Intervalo 2041-2050</t>
         </is>
       </c>
     </row>
@@ -1466,22 +1466,22 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>2015</t>
+          <t>Ano 2015</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>2030</t>
+          <t>Ano 2030</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>2040</t>
+          <t>Ano 2040</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>2050</t>
+          <t>Ano 2050</t>
         </is>
       </c>
     </row>
@@ -1550,7 +1550,7 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>2015</t>
+          <t>Ano 2015</t>
         </is>
       </c>
     </row>

</xml_diff>